<commit_message>
added missing outgroup species
</commit_message>
<xml_diff>
--- a/data/modern_samples_cattle2.xlsx
+++ b/data/modern_samples_cattle2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Evan/Dropbox/Code/alleletraj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F3A7C7-76BF-E34B-BC6F-79C46A2726EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2F44B0-2ADA-354A-9A94-04621DED7E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19660" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4393" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="1155">
   <si>
     <t>Breed</t>
   </si>
@@ -3494,6 +3494,9 @@
   </si>
   <si>
     <t>Random</t>
+  </si>
+  <si>
+    <t>TODO add 3 outgroup species</t>
   </si>
 </sst>
 </file>
@@ -3960,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J380"/>
   <sheetViews>
-    <sheetView topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15474,7 +15477,7 @@
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K33" ca="1" si="1">RAND()</f>
-        <v>0.45539107448343952</v>
+        <v>0.62536961551473036</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -15508,7 +15511,7 @@
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
-        <v>8.782557261640378E-2</v>
+        <v>0.25819564472328915</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -15542,7 +15545,7 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6726864525259137E-2</v>
+        <v>0.94926768138768447</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -15576,7 +15579,7 @@
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30312934160927563</v>
+        <v>0.62275213418572084</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -15610,7 +15613,7 @@
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33525990641118719</v>
+        <v>0.89083028782071416</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -15644,7 +15647,7 @@
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23950773773113032</v>
+        <v>0.95323600158637389</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -15678,7 +15681,7 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34557809113343974</v>
+        <v>0.36103061550724258</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -15712,7 +15715,7 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2287033295647567</v>
+        <v>0.57928254348317376</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -15746,7 +15749,7 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58068321305067627</v>
+        <v>0.95885544285106938</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -15780,7 +15783,7 @@
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66032481688714617</v>
+        <v>0.85020132151193295</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -15814,7 +15817,7 @@
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49728829945071629</v>
+        <v>0.26485617234819714</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -15848,7 +15851,7 @@
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15117278989335914</v>
+        <v>0.26168434873630086</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -15882,7 +15885,7 @@
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65453422553842033</v>
+        <v>0.44341901676128159</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -15916,7 +15919,7 @@
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46637038370513828</v>
+        <v>0.10477168271499337</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -15950,7 +15953,7 @@
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82848871313406158</v>
+        <v>0.79603882447743113</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -15984,7 +15987,7 @@
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85183710924938727</v>
+        <v>9.0757151742357323E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -16018,7 +16021,7 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44288263900953628</v>
+        <v>0.4440487783142727</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -16052,7 +16055,7 @@
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83705203699040642</v>
+        <v>0.21298719468063709</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -16086,7 +16089,7 @@
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93050820032203985</v>
+        <v>0.57583914707149575</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -16120,7 +16123,7 @@
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38426313372836385</v>
+        <v>0.2849766009358019</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -16154,7 +16157,7 @@
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2210930982601379</v>
+        <v>0.37698074551304006</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -16188,7 +16191,7 @@
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58921480634871526</v>
+        <v>0.22454604268203926</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -16222,7 +16225,7 @@
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3429750780182621</v>
+        <v>0.45309593530169368</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -16256,7 +16259,7 @@
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0121181404528592E-2</v>
+        <v>0.79194343315832305</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -16290,7 +16293,7 @@
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70914256983666735</v>
+        <v>0.91499933212258278</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -16324,7 +16327,7 @@
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46288002017397911</v>
+        <v>0.32608789683009509</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -16358,7 +16361,7 @@
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34506944573770582</v>
+        <v>0.17944214645408441</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -16392,7 +16395,7 @@
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70644868674337846</v>
+        <v>0.8827780100561875</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -16426,7 +16429,7 @@
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39086899924697593</v>
+        <v>0.27418201040569312</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -16460,7 +16463,7 @@
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60299402932580115</v>
+        <v>0.16781300851689818</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -16494,7 +16497,7 @@
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87997597106910785</v>
+        <v>0.21923274535760839</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -16528,7 +16531,7 @@
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3816203741358075E-3</v>
+        <v>0.62016791105703828</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -16562,7 +16565,7 @@
       </c>
       <c r="K34">
         <f t="shared" ref="K34:K65" ca="1" si="3">RAND()</f>
-        <v>0.99281750584442996</v>
+        <v>0.46643452108583539</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -16596,7 +16599,7 @@
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="3"/>
-        <v>0.55574173532576632</v>
+        <v>0.1641525334361349</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -16630,7 +16633,7 @@
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81020010188965852</v>
+        <v>0.32035440707731577</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -16664,7 +16667,7 @@
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="3"/>
-        <v>0.30191406907593732</v>
+        <v>0.46407765675625434</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -16698,7 +16701,7 @@
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="3"/>
-        <v>0.78074225730660973</v>
+        <v>0.59618807390124429</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -16732,7 +16735,7 @@
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5064568745768372E-2</v>
+        <v>0.36724184592919995</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -16766,7 +16769,7 @@
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="3"/>
-        <v>0.53315620215656945</v>
+        <v>2.243769876753765E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -16800,7 +16803,7 @@
       </c>
       <c r="K41">
         <f t="shared" ca="1" si="3"/>
-        <v>0.93913421792416729</v>
+        <v>0.93663566759459749</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -16834,7 +16837,7 @@
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="3"/>
-        <v>0.49222236279197518</v>
+        <v>0.44281933793306383</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -16868,7 +16871,7 @@
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16351593762414618</v>
+        <v>0.38585369251424428</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -16902,7 +16905,7 @@
       </c>
       <c r="K44">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81963739789546297</v>
+        <v>0.96887196618818028</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -16936,7 +16939,7 @@
       </c>
       <c r="K45">
         <f t="shared" ca="1" si="3"/>
-        <v>0.41106226578214844</v>
+        <v>0.58865969057611778</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -16970,7 +16973,7 @@
       </c>
       <c r="K46">
         <f t="shared" ca="1" si="3"/>
-        <v>0.71355811901882316</v>
+        <v>0.27066256762259355</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -17004,7 +17007,7 @@
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10412945668510221</v>
+        <v>0.30084742990385283</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -17038,7 +17041,7 @@
       </c>
       <c r="K48">
         <f t="shared" ca="1" si="3"/>
-        <v>0.38710719004640914</v>
+        <v>0.53156103675045951</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -17072,7 +17075,7 @@
       </c>
       <c r="K49">
         <f t="shared" ca="1" si="3"/>
-        <v>0.65607227935294721</v>
+        <v>0.36299741478743441</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -17106,7 +17109,7 @@
       </c>
       <c r="K50">
         <f t="shared" ca="1" si="3"/>
-        <v>0.61303882760166606</v>
+        <v>0.4569145369633214</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -17140,7 +17143,7 @@
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91663526932944794</v>
+        <v>0.69730370967929456</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -17174,7 +17177,7 @@
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8303689966106429E-2</v>
+        <v>0.31377413498061457</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -17208,7 +17211,7 @@
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21851481022049268</v>
+        <v>0.42618418636341893</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -17242,7 +17245,7 @@
       </c>
       <c r="K54">
         <f t="shared" ca="1" si="3"/>
-        <v>0.92910092561304625</v>
+        <v>0.14466925601848213</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -17276,7 +17279,7 @@
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="3"/>
-        <v>0.62348357768317986</v>
+        <v>0.50315074195116938</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -17310,7 +17313,7 @@
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="3"/>
-        <v>0.63270599484620393</v>
+        <v>0.35523361366387551</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -17344,7 +17347,7 @@
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87282207892322816</v>
+        <v>2.7142744975789834E-2</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -17378,7 +17381,7 @@
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="3"/>
-        <v>0.33889427109542014</v>
+        <v>7.6703073266510269E-2</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -17412,7 +17415,7 @@
       </c>
       <c r="K59">
         <f t="shared" ca="1" si="3"/>
-        <v>0.75207273531322827</v>
+        <v>0.74226884208261101</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -17446,7 +17449,7 @@
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="3"/>
-        <v>0.89963449739355017</v>
+        <v>0.27601417068905754</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -17480,7 +17483,7 @@
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="3"/>
-        <v>0.92799926293100365</v>
+        <v>0.3713181464888774</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -17514,7 +17517,7 @@
       </c>
       <c r="K62">
         <f t="shared" ca="1" si="3"/>
-        <v>0.90263462952374973</v>
+        <v>0.45552807670720052</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -17548,7 +17551,7 @@
       </c>
       <c r="K63">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16164326255128059</v>
+        <v>0.58819557963758917</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -17582,7 +17585,7 @@
       </c>
       <c r="K64">
         <f t="shared" ca="1" si="3"/>
-        <v>6.9939917964321752E-2</v>
+        <v>0.3758101709353916</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -17616,7 +17619,7 @@
       </c>
       <c r="K65">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99641793974469406</v>
+        <v>0.26566101021262511</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -17650,7 +17653,7 @@
       </c>
       <c r="K66">
         <f t="shared" ref="K66:K98" ca="1" si="5">RAND()</f>
-        <v>0.61665751253815648</v>
+        <v>0.1319577599009264</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -17684,7 +17687,7 @@
       </c>
       <c r="K67">
         <f t="shared" ca="1" si="5"/>
-        <v>0.68030394729364485</v>
+        <v>0.27996765310936644</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -17718,7 +17721,7 @@
       </c>
       <c r="K68">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99694369451915499</v>
+        <v>0.42574423106441583</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -17752,7 +17755,7 @@
       </c>
       <c r="K69">
         <f t="shared" ca="1" si="5"/>
-        <v>0.94744029586943646</v>
+        <v>0.70004376641513888</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -17786,7 +17789,7 @@
       </c>
       <c r="K70">
         <f t="shared" ca="1" si="5"/>
-        <v>0.17665225104141724</v>
+        <v>0.55916375347101444</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -17820,7 +17823,7 @@
       </c>
       <c r="K71">
         <f t="shared" ca="1" si="5"/>
-        <v>0.98695983407627064</v>
+        <v>0.75970510770798116</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -17854,7 +17857,7 @@
       </c>
       <c r="K72">
         <f t="shared" ca="1" si="5"/>
-        <v>0.67613906945760327</v>
+        <v>0.68329265329907674</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -17888,7 +17891,7 @@
       </c>
       <c r="K73">
         <f t="shared" ca="1" si="5"/>
-        <v>0.40925238069205361</v>
+        <v>0.85958441142447484</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -17922,7 +17925,7 @@
       </c>
       <c r="K74">
         <f t="shared" ca="1" si="5"/>
-        <v>0.44378688249295106</v>
+        <v>0.36120743729410398</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -17956,7 +17959,7 @@
       </c>
       <c r="K75">
         <f t="shared" ca="1" si="5"/>
-        <v>0.57975001534473936</v>
+        <v>0.58228928591131657</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -17990,7 +17993,7 @@
       </c>
       <c r="K76">
         <f t="shared" ca="1" si="5"/>
-        <v>0.14421806105619717</v>
+        <v>0.269059368891016</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -18024,7 +18027,7 @@
       </c>
       <c r="K77">
         <f t="shared" ca="1" si="5"/>
-        <v>0.70555629112635332</v>
+        <v>0.62421540292163946</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -18058,7 +18061,7 @@
       </c>
       <c r="K78">
         <f t="shared" ca="1" si="5"/>
-        <v>0.80195712111975681</v>
+        <v>0.55821284809314753</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -18092,7 +18095,7 @@
       </c>
       <c r="K79">
         <f t="shared" ca="1" si="5"/>
-        <v>0.84319030967031749</v>
+        <v>0.55753190388540841</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -18126,7 +18129,7 @@
       </c>
       <c r="K80">
         <f t="shared" ca="1" si="5"/>
-        <v>0.50553727678237659</v>
+        <v>0.54875133307450408</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -18160,7 +18163,7 @@
       </c>
       <c r="K81">
         <f t="shared" ca="1" si="5"/>
-        <v>0.77326181258699911</v>
+        <v>0.52817013005610058</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -18194,7 +18197,7 @@
       </c>
       <c r="K82">
         <f t="shared" ca="1" si="5"/>
-        <v>0.79152935792847645</v>
+        <v>0.62223731948409433</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -18228,7 +18231,7 @@
       </c>
       <c r="K83">
         <f t="shared" ca="1" si="5"/>
-        <v>0.29751988759825132</v>
+        <v>0.9220432362620169</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -18262,7 +18265,7 @@
       </c>
       <c r="K84">
         <f t="shared" ca="1" si="5"/>
-        <v>0.41932181234764998</v>
+        <v>0.75739295482270497</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -18296,7 +18299,7 @@
       </c>
       <c r="K85">
         <f t="shared" ca="1" si="5"/>
-        <v>7.5536139110886857E-2</v>
+        <v>4.5606452129592356E-2</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -18330,7 +18333,7 @@
       </c>
       <c r="K86">
         <f t="shared" ca="1" si="5"/>
-        <v>0.94210008357389241</v>
+        <v>0.11834498765630097</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -18364,7 +18367,7 @@
       </c>
       <c r="K87">
         <f t="shared" ca="1" si="5"/>
-        <v>0.53515286686580588</v>
+        <v>0.35488106032938882</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
@@ -18398,7 +18401,7 @@
       </c>
       <c r="K88">
         <f t="shared" ca="1" si="5"/>
-        <v>0.23542591191774631</v>
+        <v>0.79038835913947747</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
@@ -18432,7 +18435,7 @@
       </c>
       <c r="K89">
         <f t="shared" ca="1" si="5"/>
-        <v>0.82733997495433453</v>
+        <v>0.91245060296839242</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -18466,7 +18469,7 @@
       </c>
       <c r="K90">
         <f t="shared" ca="1" si="5"/>
-        <v>0.2576647494972415</v>
+        <v>0.32872689938057831</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -18500,7 +18503,7 @@
       </c>
       <c r="K91">
         <f t="shared" ca="1" si="5"/>
-        <v>0.87391824405762186</v>
+        <v>8.73781955114038E-2</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -18534,7 +18537,7 @@
       </c>
       <c r="K92">
         <f t="shared" ca="1" si="5"/>
-        <v>0.62817317946468276</v>
+        <v>0.42532315558686651</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -18568,7 +18571,7 @@
       </c>
       <c r="K93">
         <f t="shared" ca="1" si="5"/>
-        <v>0.187445718950354</v>
+        <v>0.82305159825851071</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -18602,7 +18605,7 @@
       </c>
       <c r="K94">
         <f t="shared" ca="1" si="5"/>
-        <v>0.95530910128443236</v>
+        <v>7.9185814278463051E-2</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -18636,7 +18639,7 @@
       </c>
       <c r="K95">
         <f t="shared" ca="1" si="5"/>
-        <v>0.99245389458052768</v>
+        <v>0.4366786760864414</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -18670,7 +18673,7 @@
       </c>
       <c r="K96">
         <f t="shared" ca="1" si="5"/>
-        <v>0.2084633851479516</v>
+        <v>0.47376225442868025</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -18704,7 +18707,7 @@
       </c>
       <c r="K97">
         <f t="shared" ca="1" si="5"/>
-        <v>0.67777792859125319</v>
+        <v>0.7322054055325129</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -18738,7 +18741,7 @@
       </c>
       <c r="K98">
         <f t="shared" ca="1" si="5"/>
-        <v>0.27207080175298981</v>
+        <v>0.46417036096729658</v>
       </c>
     </row>
   </sheetData>
@@ -18754,10 +18757,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85C35CA-E215-1A40-9762-F40E6A6D4323}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21515,6 +21518,11 @@
         <v>1152</v>
       </c>
     </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>1154</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I98" xr:uid="{D98B0F5C-0A14-E940-993A-508A1771E939}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>